<commit_message>
Asignación de autores Mat 7 tema 7
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion07/Escaleta MA_07_07_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion07/Escaleta MA_07_07_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion07\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="268">
   <si>
     <t>Asignatura</t>
   </si>
@@ -812,6 +817,18 @@
   </si>
   <si>
     <t>Magnitudes proporcionales</t>
+  </si>
+  <si>
+    <t>Adriana Lasprilla</t>
+  </si>
+  <si>
+    <t>Diana Velásquez</t>
+  </si>
+  <si>
+    <t>Johanna Vera</t>
+  </si>
+  <si>
+    <t>Clara Melo</t>
   </si>
 </sst>
 </file>
@@ -1518,6 +1535,36 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1570,36 +1617,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1662,7 +1679,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1697,7 +1714,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1906,10 +1923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U42"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C39"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="V42" sqref="V42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1932,97 +1949,97 @@
     <col min="22" max="16384" width="19.140625" style="59"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="85" t="s">
+    <row r="1" spans="1:22" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="92" t="s">
+      <c r="C1" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="103" t="s">
         <v>237</v>
       </c>
-      <c r="E1" s="95" t="s">
+      <c r="E1" s="105" t="s">
         <v>238</v>
       </c>
-      <c r="F1" s="93" t="s">
+      <c r="F1" s="103" t="s">
         <v>239</v>
       </c>
-      <c r="G1" s="91" t="s">
+      <c r="G1" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="97" t="s">
+      <c r="H1" s="107" t="s">
         <v>240</v>
       </c>
-      <c r="I1" s="99" t="s">
+      <c r="I1" s="109" t="s">
         <v>241</v>
       </c>
-      <c r="J1" s="88" t="s">
+      <c r="J1" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="87" t="s">
+      <c r="K1" s="97" t="s">
         <v>249</v>
       </c>
-      <c r="L1" s="86" t="s">
+      <c r="L1" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="89" t="s">
+      <c r="M1" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="90"/>
-      <c r="O1" s="83" t="s">
+      <c r="N1" s="100"/>
+      <c r="O1" s="93" t="s">
         <v>99</v>
       </c>
-      <c r="P1" s="101" t="s">
+      <c r="P1" s="83" t="s">
         <v>242</v>
       </c>
-      <c r="Q1" s="102" t="s">
+      <c r="Q1" s="84" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="108" t="s">
+      <c r="R1" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="S1" s="106" t="s">
+      <c r="S1" s="88" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="104" t="s">
+      <c r="T1" s="86" t="s">
         <v>90</v>
       </c>
-      <c r="U1" s="102" t="s">
+      <c r="U1" s="84" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="85"/>
-      <c r="B2" s="84"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="86"/>
+    <row r="2" spans="1:22" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="95"/>
+      <c r="B2" s="94"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="96"/>
       <c r="M2" s="30" t="s">
         <v>92</v>
       </c>
       <c r="N2" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="83"/>
-      <c r="P2" s="101"/>
-      <c r="Q2" s="110"/>
-      <c r="R2" s="109"/>
-      <c r="S2" s="107"/>
-      <c r="T2" s="105"/>
-      <c r="U2" s="103"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="O2" s="93"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="92"/>
+      <c r="R2" s="91"/>
+      <c r="S2" s="89"/>
+      <c r="T2" s="87"/>
+      <c r="U2" s="85"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>74</v>
       </c>
@@ -2082,8 +2099,11 @@
       <c r="U3" s="42" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V3" s="59" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
         <v>74</v>
       </c>
@@ -2137,8 +2157,11 @@
       <c r="U4" s="46" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V4" s="59" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
         <v>74</v>
       </c>
@@ -2198,8 +2221,11 @@
       <c r="U5" s="51" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V5" s="59" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
         <v>74</v>
       </c>
@@ -2255,8 +2281,11 @@
       <c r="U6" s="52" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V6" s="59" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
         <v>74</v>
       </c>
@@ -2312,8 +2341,11 @@
       <c r="U7" s="54" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V7" s="59" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="31" t="s">
         <v>74</v>
       </c>
@@ -2369,8 +2401,11 @@
       <c r="U8" s="54" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V8" s="59" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
         <v>74</v>
       </c>
@@ -2429,7 +2464,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
         <v>74</v>
       </c>
@@ -2484,7 +2519,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="31" t="s">
         <v>74</v>
       </c>
@@ -2544,8 +2579,11 @@
       <c r="U11" s="54" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V11" s="59" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
         <v>74</v>
       </c>
@@ -2600,7 +2638,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
         <v>74</v>
       </c>
@@ -2658,8 +2696,11 @@
       <c r="U13" s="54" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V13" s="59" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
         <v>74</v>
       </c>
@@ -2719,8 +2760,11 @@
       <c r="U14" s="54" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V14" s="59" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
         <v>74</v>
       </c>
@@ -2775,7 +2819,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="31" t="s">
         <v>74</v>
       </c>
@@ -2833,8 +2877,11 @@
       <c r="U16" s="54" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V16" s="59" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="31" t="s">
         <v>74</v>
       </c>
@@ -2893,7 +2940,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="31" t="s">
         <v>74</v>
       </c>
@@ -2951,8 +2998,11 @@
       <c r="U18" s="54" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V18" s="59" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="31" t="s">
         <v>74</v>
       </c>
@@ -3007,7 +3057,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="31" t="s">
         <v>74</v>
       </c>
@@ -3066,7 +3116,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="31" t="s">
         <v>74</v>
       </c>
@@ -3126,8 +3176,11 @@
       <c r="U21" s="54" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V21" s="59" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="31" t="s">
         <v>74</v>
       </c>
@@ -3187,8 +3240,11 @@
       <c r="U22" s="54" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V22" s="59" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="31" t="s">
         <v>74</v>
       </c>
@@ -3248,8 +3304,11 @@
       <c r="U23" s="54" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V23" s="59" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="31" t="s">
         <v>74</v>
       </c>
@@ -3307,8 +3366,11 @@
       <c r="U24" s="54" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V24" s="59" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="31" t="s">
         <v>74</v>
       </c>
@@ -3368,8 +3430,11 @@
       <c r="U25" s="54" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V25" s="59" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="31" t="s">
         <v>74</v>
       </c>
@@ -3428,7 +3493,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="31" t="s">
         <v>74</v>
       </c>
@@ -3488,8 +3553,11 @@
       <c r="U27" s="54" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V27" s="59" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="31" t="s">
         <v>74</v>
       </c>
@@ -3547,8 +3615,11 @@
       <c r="U28" s="54" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V28" s="59" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="31" t="s">
         <v>74</v>
       </c>
@@ -3608,8 +3679,11 @@
       <c r="U29" s="54" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V29" s="59" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="31" t="s">
         <v>74</v>
       </c>
@@ -3664,7 +3738,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="31" t="s">
         <v>74</v>
       </c>
@@ -3719,7 +3793,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="31" t="s">
         <v>74</v>
       </c>
@@ -3779,8 +3853,11 @@
       <c r="U32" s="54" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V32" s="59" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" s="31" t="s">
         <v>74</v>
       </c>
@@ -3837,7 +3914,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="31" t="s">
         <v>74</v>
       </c>
@@ -3895,8 +3972,11 @@
       <c r="U34" s="54" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V34" s="59" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="31" t="s">
         <v>74</v>
       </c>
@@ -3956,8 +4036,11 @@
       <c r="U35" s="54" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V35" s="59" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" s="31" t="s">
         <v>74</v>
       </c>
@@ -4012,7 +4095,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" s="31" t="s">
         <v>74</v>
       </c>
@@ -4059,7 +4142,7 @@
       <c r="T37" s="82"/>
       <c r="U37" s="54"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" s="31" t="s">
         <v>74</v>
       </c>
@@ -4117,8 +4200,11 @@
       <c r="U38" s="54" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V38" s="59" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" s="31" t="s">
         <v>74</v>
       </c>
@@ -4174,18 +4260,15 @@
       <c r="U39" s="54" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V39" s="59" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D42" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
@@ -4200,9 +4283,15 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P4 V25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P4">
       <formula1>$W$27:$W$27</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K39">

</xml_diff>